<commit_message>
mostly worked on abstracts including ms abstract
</commit_message>
<xml_diff>
--- a/author_info.xlsx
+++ b/author_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Liu</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">liumolm@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">0000-0001-5990-6585</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huang</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t xml:space="preserve">261565020@qq.com</t>
   </si>
   <si>
+    <t xml:space="preserve">0000-0002-7669-7364</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wu</t>
   </si>
   <si>
@@ -49,6 +55,9 @@
     <t xml:space="preserve">wuxm8523@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">0009-0000-8247-7432</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zheng</t>
   </si>
   <si>
@@ -58,6 +67,9 @@
     <t xml:space="preserve">zhengqi2727@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">0009-0007-7427-9437</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yao</t>
   </si>
   <si>
@@ -67,6 +79,9 @@
     <t xml:space="preserve">yaort@mail2.sysu.edu.cn</t>
   </si>
   <si>
+    <t xml:space="preserve">0009-0006-5483-3667</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yang</t>
   </si>
   <si>
@@ -74,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yangying@163.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0009-0000-0309-0353 </t>
   </si>
   <si>
     <t xml:space="preserve">Shen</t>
@@ -128,12 +146,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -155,20 +172,11 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,16 +230,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -357,15 +365,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,115 +387,133 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>